<commit_message>
corrected engineering reference designator
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE06ISSP_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CE06ISSP_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\# OOI_Asset_Management\CE_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="852" yWindow="840" windowWidth="25608" windowHeight="16068" tabRatio="579"/>
+    <workbookView xWindow="855" yWindow="840" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="114">
   <si>
     <t>Ref Des</t>
   </si>
@@ -2239,28 +2239,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -2341,25 +2341,25 @@
         <v>-124.27325999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
       <c r="F4" s="12"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
@@ -2368,7 +2368,7 @@
         <v>47.134799999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="12"/>
@@ -2377,61 +2377,61 @@
         <v>-124.27325999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
       <c r="F8" s="12"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D10" s="10"/>
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:14" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="4:7" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -2455,23 +2455,23 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="5" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" style="7" customWidth="1"/>
-    <col min="7" max="7" width="37.88671875" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2511,7 +2511,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>68</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>68</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>68</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>68</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="23"/>
@@ -2638,7 +2638,7 @@
       <c r="H7" s="21"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>67</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>67</v>
       </c>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="I9" s="27"/>
     </row>
-    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>67</v>
       </c>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="I10" s="27"/>
     </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>67</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="I11" s="27"/>
     </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>67</v>
       </c>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>67</v>
       </c>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="I13" s="27"/>
     </row>
-    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>67</v>
       </c>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="I14" s="27"/>
     </row>
-    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>67</v>
       </c>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="I15" s="27"/>
     </row>
-    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="23"/>
@@ -2867,7 +2867,7 @@
       <c r="H16" s="21"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>69</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>69</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="23"/>
@@ -2936,7 +2936,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>70</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>70</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>70</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>70</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>70</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>70</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>70</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="23"/>
@@ -3150,7 +3150,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>71</v>
       </c>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>71</v>
       </c>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>71</v>
       </c>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="23"/>
@@ -3242,7 +3242,7 @@
       <c r="H31" s="21"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>72</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>72</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>72</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>72</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>72</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>72</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>72</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>72</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>72</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>72</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="22"/>
       <c r="C42" s="23"/>
@@ -3543,7 +3543,7 @@
       <c r="H42" s="21"/>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>73</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>73</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="23"/>
@@ -3612,7 +3612,7 @@
       <c r="H45" s="21"/>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>74</v>
       </c>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="I46" s="16"/>
     </row>
-    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>74</v>
       </c>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="I47" s="16"/>
     </row>
-    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>74</v>
       </c>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A49" s="29"/>
       <c r="B49" s="29"/>
       <c r="C49" s="29"/>
@@ -3704,11 +3704,13 @@
       <c r="H49" s="30"/>
       <c r="I49" s="29"/>
     </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="31"/>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
       <c r="C50" s="19" t="s">
         <v>65</v>
       </c>
@@ -3725,10 +3727,10 @@
       <c r="H50" s="32"/>
       <c r="I50" s="16"/>
     </row>
-    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3749,9 +3751,9 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-2.5780999999999998E-2</v>
       </c>
@@ -3858,7 +3860,7 @@
         <v>2.1193E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1.7167999999999999E-2</v>
       </c>
@@ -3965,7 +3967,7 @@
         <v>1.1336000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-8.5559999999999994E-3</v>
       </c>
@@ -4072,7 +4074,7 @@
         <v>2.3340000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.0000000000000002E-5</v>
       </c>
@@ -4179,7 +4181,7 @@
         <v>-4.3610000000000003E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.117E-3</v>
       </c>
@@ -4286,7 +4288,7 @@
         <v>-7.6249999999999998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.182E-3</v>
       </c>
@@ -4393,7 +4395,7 @@
         <v>-9.7070000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.6540000000000002E-3</v>
       </c>
@@ -4500,7 +4502,7 @@
         <v>-1.0126E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.8370000000000001E-3</v>
       </c>
@@ -4607,7 +4609,7 @@
         <v>-9.5200000000000007E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.9389999999999998E-3</v>
       </c>
@@ -4714,7 +4716,7 @@
         <v>-9.9399999999999992E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.679E-3</v>
       </c>
@@ -4821,7 +4823,7 @@
         <v>-9.6399999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7.9609999999999993E-3</v>
       </c>
@@ -4928,7 +4930,7 @@
         <v>-9.2029999999999994E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8.8800000000000007E-3</v>
       </c>
@@ -5035,7 +5037,7 @@
         <v>-8.9390000000000008E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9.4479999999999998E-3</v>
       </c>
@@ -5142,7 +5144,7 @@
         <v>-8.8070000000000006E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9.8200000000000006E-3</v>
       </c>
@@ -5249,7 +5251,7 @@
         <v>-8.3180000000000007E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.0178E-2</v>
       </c>
@@ -5356,7 +5358,7 @@
         <v>-8.3160000000000005E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.1164E-2</v>
       </c>
@@ -5463,7 +5465,7 @@
         <v>-7.9609999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.1211E-2</v>
       </c>
@@ -5570,7 +5572,7 @@
         <v>-7.6880000000000004E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.0957E-2</v>
       </c>
@@ -5677,7 +5679,7 @@
         <v>-7.3470000000000002E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.0567E-2</v>
       </c>
@@ -5784,7 +5786,7 @@
         <v>-7.0359999999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9.6740000000000003E-3</v>
       </c>
@@ -5891,7 +5893,7 @@
         <v>-6.6239999999999997E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9.3410000000000003E-3</v>
       </c>
@@ -5998,7 +6000,7 @@
         <v>-6.306E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8.4539999999999997E-3</v>
       </c>
@@ -6105,7 +6107,7 @@
         <v>-5.8950000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8.2310000000000005E-3</v>
       </c>
@@ -6212,7 +6214,7 @@
         <v>-5.509E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7.3109999999999998E-3</v>
       </c>
@@ -6319,7 +6321,7 @@
         <v>-5.019E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6.7530000000000003E-3</v>
       </c>
@@ -6426,7 +6428,7 @@
         <v>-4.646E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6.3889999999999997E-3</v>
       </c>
@@ -6533,7 +6535,7 @@
         <v>-4.2750000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5.8970000000000003E-3</v>
       </c>
@@ -6640,7 +6642,7 @@
         <v>-3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5.5420000000000001E-3</v>
       </c>
@@ -6747,7 +6749,7 @@
         <v>-3.4640000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4.9880000000000002E-3</v>
       </c>
@@ -6854,7 +6856,7 @@
         <v>-3.1089999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4.999E-3</v>
       </c>
@@ -6961,7 +6963,7 @@
         <v>-2.807E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4.6410000000000002E-3</v>
       </c>
@@ -7068,7 +7070,7 @@
         <v>-2.444E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4.5269999999999998E-3</v>
       </c>
@@ -7175,7 +7177,7 @@
         <v>-2.173E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4.1970000000000002E-3</v>
       </c>
@@ -7282,7 +7284,7 @@
         <v>-1.92E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3.8089999999999999E-3</v>
       </c>
@@ -7389,7 +7391,7 @@
         <v>-1.7129999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3.189E-3</v>
       </c>
@@ -7496,7 +7498,7 @@
         <v>-1.567E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2.2560000000000002E-3</v>
       </c>
@@ -7603,7 +7605,7 @@
         <v>-1.438E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.147E-3</v>
       </c>
@@ -7710,7 +7712,7 @@
         <v>-1.341E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-4.4700000000000002E-4</v>
       </c>
@@ -7817,7 +7819,7 @@
         <v>-1.328E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-2.1570000000000001E-3</v>
       </c>
@@ -7924,7 +7926,7 @@
         <v>-1.4239999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-3.0799999999999998E-3</v>
       </c>
@@ -8031,7 +8033,7 @@
         <v>-1.467E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-3.5469999999999998E-3</v>
       </c>
@@ -8138,7 +8140,7 @@
         <v>-1.64E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-3.1150000000000001E-3</v>
       </c>
@@ -8245,7 +8247,7 @@
         <v>-1.7359999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-5.0340000000000003E-3</v>
       </c>
@@ -8352,7 +8354,7 @@
         <v>-7.4200000000000004E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-4.5750000000000001E-3</v>
       </c>
@@ -8459,7 +8461,7 @@
         <v>-7.5600000000000005E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-4.5779999999999996E-3</v>
       </c>
@@ -8566,7 +8568,7 @@
         <v>-7.2400000000000003E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-4.176E-3</v>
       </c>
@@ -8673,7 +8675,7 @@
         <v>-7.2400000000000003E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-4.071E-3</v>
       </c>
@@ -8780,7 +8782,7 @@
         <v>-7.6000000000000004E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-3.8679999999999999E-3</v>
       </c>
@@ -8887,7 +8889,7 @@
         <v>-7.8799999999999996E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-3.5279999999999999E-3</v>
       </c>
@@ -8994,7 +8996,7 @@
         <v>-7.8100000000000001E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-3.3969999999999998E-3</v>
       </c>
@@ -9101,7 +9103,7 @@
         <v>-7.6999999999999996E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-3.4169999999999999E-3</v>
       </c>
@@ -9208,7 +9210,7 @@
         <v>-7.94E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-3.483E-3</v>
       </c>
@@ -9315,7 +9317,7 @@
         <v>-7.9100000000000004E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-3.454E-3</v>
       </c>
@@ -9422,7 +9424,7 @@
         <v>-7.2199999999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-3.4759999999999999E-3</v>
       </c>
@@ -9529,7 +9531,7 @@
         <v>-7.1699999999999997E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-3.5729999999999998E-3</v>
       </c>
@@ -9636,7 +9638,7 @@
         <v>-7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-3.666E-3</v>
       </c>
@@ -9743,7 +9745,7 @@
         <v>-6.5499999999999998E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-3.771E-3</v>
       </c>
@@ -9850,7 +9852,7 @@
         <v>-6.4599999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-3.8969999999999999E-3</v>
       </c>
@@ -9957,7 +9959,7 @@
         <v>-6.0800000000000003E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-4.0460000000000001E-3</v>
       </c>
@@ -10064,7 +10066,7 @@
         <v>-6.0599999999999998E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-4.1229999999999999E-3</v>
       </c>
@@ -10171,7 +10173,7 @@
         <v>-5.71E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-4.4140000000000004E-3</v>
       </c>
@@ -10278,7 +10280,7 @@
         <v>-5.0500000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-4.5139999999999998E-3</v>
       </c>
@@ -10385,7 +10387,7 @@
         <v>-4.6500000000000003E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-4.5279999999999999E-3</v>
       </c>
@@ -10492,7 +10494,7 @@
         <v>-4.3399999999999998E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-4.7699999999999999E-3</v>
       </c>
@@ -10599,7 +10601,7 @@
         <v>-4.0299999999999998E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-4.6909999999999999E-3</v>
       </c>
@@ -10706,7 +10708,7 @@
         <v>-3.4900000000000003E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-4.9100000000000003E-3</v>
       </c>
@@ -10813,7 +10815,7 @@
         <v>-3.3E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-4.9040000000000004E-3</v>
       </c>
@@ -10920,7 +10922,7 @@
         <v>-3.1199999999999999E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-4.9459999999999999E-3</v>
       </c>
@@ -11027,7 +11029,7 @@
         <v>-3.1500000000000001E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-5.2160000000000002E-3</v>
       </c>
@@ -11134,7 +11136,7 @@
         <v>-2.9100000000000003E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-5.1619999999999999E-3</v>
       </c>
@@ -11241,7 +11243,7 @@
         <v>-2.5099999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-5.267E-3</v>
       </c>
@@ -11348,7 +11350,7 @@
         <v>-2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-5.3049999999999998E-3</v>
       </c>
@@ -11455,7 +11457,7 @@
         <v>-2.6699999999999998E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-5.1419999999999999E-3</v>
       </c>
@@ -11562,7 +11564,7 @@
         <v>-2.6699999999999998E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-5.0359999999999997E-3</v>
       </c>
@@ -11669,7 +11671,7 @@
         <v>-1.83E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-5.3579999999999999E-3</v>
       </c>
@@ -11776,7 +11778,7 @@
         <v>-7.7999999999999999E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-5.3299999999999997E-3</v>
       </c>
@@ -11883,7 +11885,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-5.3070000000000001E-3</v>
       </c>
@@ -11990,7 +11992,7 @@
         <v>7.6000000000000004E-5</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-5.2009999999999999E-3</v>
       </c>
@@ -12097,7 +12099,7 @@
         <v>1.05E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-4.8599999999999997E-3</v>
       </c>
@@ -12204,7 +12206,7 @@
         <v>1.8900000000000001E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-4.6449999999999998E-3</v>
       </c>
@@ -12311,7 +12313,7 @@
         <v>1.3899999999999999E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-4.365E-3</v>
       </c>
@@ -12418,7 +12420,7 @@
         <v>2.02E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-4.7549999999999997E-3</v>
       </c>
@@ -12525,7 +12527,7 @@
         <v>2.1100000000000001E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-4.6899999999999997E-3</v>
       </c>
@@ -12632,7 +12634,7 @@
         <v>3.3199999999999999E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-5.0220000000000004E-3</v>
       </c>
@@ -12739,7 +12741,7 @@
         <v>3.7100000000000002E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-5.5160000000000001E-3</v>
       </c>
@@ -12864,9 +12866,9 @@
       <selection sqref="A1:AI85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-4.1287999999999998E-2</v>
       </c>
@@ -12973,7 +12975,7 @@
         <v>-1.4790000000000001E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-4.1367000000000001E-2</v>
       </c>
@@ -13080,7 +13082,7 @@
         <v>-2.611E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-3.7718000000000002E-2</v>
       </c>
@@ -13187,7 +13189,7 @@
         <v>-1.418E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-3.5545E-2</v>
       </c>
@@ -13294,7 +13296,7 @@
         <v>-2.5010000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-3.0488999999999999E-2</v>
       </c>
@@ -13401,7 +13403,7 @@
         <v>-2.6819999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-2.7740999999999998E-2</v>
       </c>
@@ -13508,7 +13510,7 @@
         <v>-3.4970000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-2.4542999999999999E-2</v>
       </c>
@@ -13615,7 +13617,7 @@
         <v>-2.663E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-2.3806999999999998E-2</v>
       </c>
@@ -13722,7 +13724,7 @@
         <v>-3.852E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-2.1422E-2</v>
       </c>
@@ -13829,7 +13831,7 @@
         <v>-4.0220000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-2.0753000000000001E-2</v>
       </c>
@@ -13936,7 +13938,7 @@
         <v>-4.2459999999999998E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-1.8873999999999998E-2</v>
       </c>
@@ -14043,7 +14045,7 @@
         <v>-3.9769999999999996E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1.8828999999999999E-2</v>
       </c>
@@ -14150,7 +14152,7 @@
         <v>-4.2550000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-1.8471000000000001E-2</v>
       </c>
@@ -14257,7 +14259,7 @@
         <v>-4.2909999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-1.7864000000000001E-2</v>
       </c>
@@ -14364,7 +14366,7 @@
         <v>-4.2659999999999998E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-1.7205000000000002E-2</v>
       </c>
@@ -14471,7 +14473,7 @@
         <v>-4.1949999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-1.7103E-2</v>
       </c>
@@ -14578,7 +14580,7 @@
         <v>-4.1640000000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-1.6115999999999998E-2</v>
       </c>
@@ -14685,7 +14687,7 @@
         <v>-4.267E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-1.5507E-2</v>
       </c>
@@ -14792,7 +14794,7 @@
         <v>-4.1989999999999996E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-1.473E-2</v>
       </c>
@@ -14899,7 +14901,7 @@
         <v>-4.15E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-1.3806000000000001E-2</v>
       </c>
@@ -15006,7 +15008,7 @@
         <v>-4.0239999999999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-1.2939000000000001E-2</v>
       </c>
@@ -15113,7 +15115,7 @@
         <v>-4.0619999999999996E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-1.2475E-2</v>
       </c>
@@ -15220,7 +15222,7 @@
         <v>-3.9150000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-1.1646999999999999E-2</v>
       </c>
@@ -15327,7 +15329,7 @@
         <v>-3.954E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-1.0881E-2</v>
       </c>
@@ -15434,7 +15436,7 @@
         <v>-4.0109999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1.0399E-2</v>
       </c>
@@ -15541,7 +15543,7 @@
         <v>-3.8639999999999998E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-9.9030000000000003E-3</v>
       </c>
@@ -15648,7 +15650,7 @@
         <v>-3.8570000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9.4710000000000003E-3</v>
       </c>
@@ -15755,7 +15757,7 @@
         <v>-3.7780000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8.8470000000000007E-3</v>
       </c>
@@ -15862,7 +15864,7 @@
         <v>-3.908E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-8.4019999999999997E-3</v>
       </c>
@@ -15969,7 +15971,7 @@
         <v>-3.8609999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-7.5960000000000003E-3</v>
       </c>
@@ -16076,7 +16078,7 @@
         <v>-3.7320000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-7.1190000000000003E-3</v>
       </c>
@@ -16183,7 +16185,7 @@
         <v>-3.8119999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-6.5079999999999999E-3</v>
       </c>
@@ -16290,7 +16292,7 @@
         <v>-3.8159999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-5.9249999999999997E-3</v>
       </c>
@@ -16397,7 +16399,7 @@
         <v>-3.7580000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-5.1320000000000003E-3</v>
       </c>
@@ -16504,7 +16506,7 @@
         <v>-3.6679999999999998E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-4.8580000000000003E-3</v>
       </c>
@@ -16611,7 +16613,7 @@
         <v>-3.5309999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-4.9160000000000002E-3</v>
       </c>
@@ -16718,7 +16720,7 @@
         <v>-3.421E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-5.2449999999999997E-3</v>
       </c>
@@ -16825,7 +16827,7 @@
         <v>-3.2940000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-5.8999999999999999E-3</v>
       </c>
@@ -16932,7 +16934,7 @@
         <v>-3.0309999999999998E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-6.7629999999999999E-3</v>
       </c>
@@ -17039,7 +17041,7 @@
         <v>-2.8449999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-7.8220000000000008E-3</v>
       </c>
@@ -17146,7 +17148,7 @@
         <v>-2.6319999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-8.6490000000000004E-3</v>
       </c>
@@ -17253,7 +17255,7 @@
         <v>-2.4719999999999998E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-9.639E-3</v>
       </c>
@@ -17360,7 +17362,7 @@
         <v>-2.3349999999999998E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-9.6080000000000002E-3</v>
       </c>
@@ -17467,7 +17469,7 @@
         <v>-1.536E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-9.6089999999999995E-3</v>
       </c>
@@ -17574,7 +17576,7 @@
         <v>-1.469E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-9.2999999999999992E-3</v>
       </c>
@@ -17681,7 +17683,7 @@
         <v>-1.469E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-8.9479999999999994E-3</v>
       </c>
@@ -17788,7 +17790,7 @@
         <v>-1.4809999999999999E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-9.0410000000000004E-3</v>
       </c>
@@ -17895,7 +17897,7 @@
         <v>-1.5330000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-8.6440000000000006E-3</v>
       </c>
@@ -18002,7 +18004,7 @@
         <v>-1.555E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-8.4069999999999995E-3</v>
       </c>
@@ -18109,7 +18111,7 @@
         <v>-1.66E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-8.2459999999999999E-3</v>
       </c>
@@ -18216,7 +18218,7 @@
         <v>-1.7489999999999999E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-8.064E-3</v>
       </c>
@@ -18323,7 +18325,7 @@
         <v>-1.7750000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-8.2019999999999992E-3</v>
       </c>
@@ -18430,7 +18432,7 @@
         <v>-1.8450000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-8.0560000000000007E-3</v>
       </c>
@@ -18537,7 +18539,7 @@
         <v>-1.902E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-7.9369999999999996E-3</v>
       </c>
@@ -18644,7 +18646,7 @@
         <v>-1.933E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-7.9690000000000004E-3</v>
       </c>
@@ -18751,7 +18753,7 @@
         <v>-1.97E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-7.7330000000000003E-3</v>
       </c>
@@ -18858,7 +18860,7 @@
         <v>-2.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-7.7270000000000004E-3</v>
       </c>
@@ -18965,7 +18967,7 @@
         <v>-2.055E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-7.705E-3</v>
       </c>
@@ -19072,7 +19074,7 @@
         <v>-2.088E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-7.4609999999999998E-3</v>
       </c>
@@ -19179,7 +19181,7 @@
         <v>-2.1220000000000002E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-7.3410000000000003E-3</v>
       </c>
@@ -19286,7 +19288,7 @@
         <v>-2.1619999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-7.3309999999999998E-3</v>
       </c>
@@ -19393,7 +19395,7 @@
         <v>-2.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-7.1980000000000004E-3</v>
       </c>
@@ -19500,7 +19502,7 @@
         <v>-2.1710000000000002E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-7.2509999999999996E-3</v>
       </c>
@@ -19607,7 +19609,7 @@
         <v>-2.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-7.1089999999999999E-3</v>
       </c>
@@ -19714,7 +19716,7 @@
         <v>-2.2799999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-6.8580000000000004E-3</v>
       </c>
@@ -19821,7 +19823,7 @@
         <v>-2.3530000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-6.986E-3</v>
       </c>
@@ -19928,7 +19930,7 @@
         <v>-2.4290000000000002E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-6.9249999999999997E-3</v>
       </c>
@@ -20035,7 +20037,7 @@
         <v>-2.5379999999999999E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-6.7470000000000004E-3</v>
       </c>
@@ -20142,7 +20144,7 @@
         <v>-2.5509999999999999E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-6.8209999999999998E-3</v>
       </c>
@@ -20249,7 +20251,7 @@
         <v>-2.6580000000000002E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-6.6490000000000004E-3</v>
       </c>
@@ -20356,7 +20358,7 @@
         <v>-2.6949999999999999E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-6.4850000000000003E-3</v>
       </c>
@@ -20463,7 +20465,7 @@
         <v>-2.7950000000000002E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-6.3400000000000001E-3</v>
       </c>
@@ -20570,7 +20572,7 @@
         <v>-2.9629999999999999E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-6.1980000000000004E-3</v>
       </c>
@@ -20677,7 +20679,7 @@
         <v>-2.9659999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-6.0150000000000004E-3</v>
       </c>
@@ -20784,7 +20786,7 @@
         <v>-2.9949999999999998E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-5.9810000000000002E-3</v>
       </c>
@@ -20891,7 +20893,7 @@
         <v>-3.068E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-6.1799999999999997E-3</v>
       </c>
@@ -20998,7 +21000,7 @@
         <v>-3.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-6.1149999999999998E-3</v>
       </c>
@@ -21105,7 +21107,7 @@
         <v>-2.905E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-6.5690000000000002E-3</v>
       </c>
@@ -21212,7 +21214,7 @@
         <v>-2.8839999999999998E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-6.6020000000000002E-3</v>
       </c>
@@ -21319,7 +21321,7 @@
         <v>-2.7650000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-6.3099999999999996E-3</v>
       </c>
@@ -21426,7 +21428,7 @@
         <v>-2.6740000000000002E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-6.2199999999999998E-3</v>
       </c>
@@ -21533,7 +21535,7 @@
         <v>-2.6849999999999999E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-5.9670000000000001E-3</v>
       </c>
@@ -21640,7 +21642,7 @@
         <v>-2.689E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-5.4429999999999999E-3</v>
       </c>
@@ -21747,7 +21749,7 @@
         <v>-2.6489999999999999E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-4.9690000000000003E-3</v>
       </c>
@@ -21854,7 +21856,7 @@
         <v>-2.761E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-5.0340000000000003E-3</v>
       </c>

</xml_diff>